<commit_message>
création d'un alerte quand on créé un fichier de données
</commit_message>
<xml_diff>
--- a/nouveauFichier.xlsx
+++ b/nouveauFichier.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -38,16 +38,16 @@
     <t>TYPE</t>
   </si>
   <si>
-    <t>Chris</t>
-  </si>
-  <si>
-    <t>Jordan</t>
+    <t>Njohou</t>
+  </si>
+  <si>
+    <t>Landry</t>
   </si>
   <si>
     <t>2021-02-01</t>
   </si>
   <si>
-    <t>Mathematique</t>
+    <t>Maths</t>
   </si>
   <si>
     <t>semestre 1</t>
@@ -56,7 +56,28 @@
     <t>Présent(e)</t>
   </si>
   <si>
-    <t>2020-12-15</t>
+    <t>Nkoa</t>
+  </si>
+  <si>
+    <t>Christophe</t>
+  </si>
+  <si>
+    <t>2021-01-30</t>
+  </si>
+  <si>
+    <t>Electronique</t>
+  </si>
+  <si>
+    <t>semestre 2</t>
+  </si>
+  <si>
+    <t>En retard</t>
+  </si>
+  <si>
+    <t>2021-02-04</t>
+  </si>
+  <si>
+    <t>2021-01-14</t>
   </si>
   <si>
     <t>Absent(e)</t>
@@ -110,7 +131,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -173,25 +194,77 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2019.0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2021.0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2019.0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2019.0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>